<commit_message>
Korrektur U5 und U35
</commit_message>
<xml_diff>
--- a/Teleskop-Kamera-Effizienz.xlsx
+++ b/Teleskop-Kamera-Effizienz.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WFS\AG-Astro-Praxis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB32BBC-2273-436B-933D-8C030269C66B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51EC35AB-B60B-430A-9F93-2D5DF8EDCD00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29625" yWindow="0" windowWidth="27525" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="75er RC WFS" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U37" authorId="0" shapeId="0" xr:uid="{1C4C1AAA-D003-48F6-9ED9-9A4D294B3357}">
+    <comment ref="U42" authorId="0" shapeId="0" xr:uid="{1C4C1AAA-D003-48F6-9ED9-9A4D294B3357}">
       <text>
         <r>
           <rPr>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="39">
   <si>
     <t>Teleskop</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>Die Tabelle zeigt die Abhängigkeiten von  Teleskop-Größen, Pixelgröße und Binning  auf die Effizenz (was hinten rauskommt) eines Teleskops am Beispiel des 75cm-RCs der WFS und anderen Teleskopen zum Vergleich</t>
+  </si>
+  <si>
+    <t>FLI-PL23042</t>
   </si>
   <si>
     <r>
@@ -251,7 +254,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>U30.</t>
+      <t>U35</t>
     </r>
   </si>
 </sst>
@@ -733,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X40"/>
+  <dimension ref="A1:X45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,7 +762,7 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
@@ -2607,15 +2610,27 @@
         <v>8483712.3000000007</v>
       </c>
     </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="E29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="Q29" s="8"/>
+      <c r="R29" s="12"/>
+      <c r="S29" s="11"/>
+      <c r="T29" s="12"/>
+      <c r="U29" s="8"/>
+      <c r="V29" s="7"/>
+      <c r="W29" s="7"/>
+      <c r="X29" s="7"/>
+    </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B30">
-        <v>300</v>
+        <v>750</v>
       </c>
       <c r="C30">
-        <v>2400</v>
+        <v>5600</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -2624,85 +2639,85 @@
         <v>0.5</v>
       </c>
       <c r="F30" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="G30" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H30">
         <v>16</v>
       </c>
       <c r="I30">
-        <v>6248</v>
+        <v>2048</v>
       </c>
       <c r="J30">
-        <v>4176</v>
+        <v>2048</v>
       </c>
       <c r="K30">
-        <v>3.75</v>
+        <v>15</v>
       </c>
       <c r="L30" s="2">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="M30">
         <f>ROUND(3.14*(B30/2)^2,1)</f>
-        <v>70650</v>
+        <v>441562.5</v>
       </c>
       <c r="N30">
         <f>ROUND(3.14*(B30*E30/2)^2,1)</f>
-        <v>17662.5</v>
+        <v>110390.6</v>
       </c>
       <c r="O30">
         <f>ROUND(SQRT((M30-N30)/3.14)*2,1)</f>
-        <v>259.8</v>
+        <v>649.5</v>
       </c>
       <c r="P30">
         <f>ROUND(C30/B30,2)</f>
-        <v>8</v>
+        <v>7.47</v>
       </c>
       <c r="Q30" s="3">
         <f>ROUND(K30/(C30/206),2)</f>
-        <v>0.32</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R30" s="4">
         <f>2*Q30</f>
-        <v>0.64</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="S30" s="4">
         <f>3*Q30</f>
-        <v>0.96</v>
+        <v>1.6500000000000001</v>
       </c>
       <c r="T30" s="4">
         <f>4*Q30</f>
-        <v>1.28</v>
-      </c>
-      <c r="U30" s="15">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="U30" s="7">
         <f>ROUND(O30^2*Q30^2*L30,1)</f>
-        <v>5529.3</v>
+        <v>121229.2</v>
       </c>
       <c r="V30" s="8">
         <f>ROUND(O30^2*R30^2*L30,1)</f>
-        <v>22117.1</v>
+        <v>484916.9</v>
       </c>
       <c r="W30" s="8">
         <f>ROUND(O30^2*S30^2*L30,1)</f>
-        <v>49763.5</v>
+        <v>1091062.8999999999</v>
       </c>
       <c r="X30" s="8">
         <f>ROUND(O30^2*T30^2*L30,1)</f>
-        <v>88468.4</v>
+        <v>1939667.4</v>
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B31">
-        <v>300</v>
+        <v>750</v>
       </c>
       <c r="C31">
         <f>C30*D31</f>
-        <v>1608</v>
+        <v>3752</v>
       </c>
       <c r="D31">
         <v>0.67</v>
@@ -2711,263 +2726,351 @@
         <v>0.5</v>
       </c>
       <c r="F31" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="G31" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H31">
         <v>16</v>
       </c>
       <c r="I31">
-        <v>6248</v>
+        <v>2048</v>
       </c>
       <c r="J31">
-        <v>4176</v>
+        <v>2048</v>
       </c>
       <c r="K31">
-        <v>3.75</v>
+        <v>15</v>
       </c>
       <c r="L31" s="2">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="M31">
         <f>ROUND(3.14*(B31/2)^2,1)</f>
-        <v>70650</v>
+        <v>441562.5</v>
       </c>
       <c r="N31">
         <f>ROUND(3.14*(B31*E31/2)^2,1)</f>
-        <v>17662.5</v>
+        <v>110390.6</v>
       </c>
       <c r="O31">
-        <f t="shared" ref="O31" si="45">ROUND(SQRT((M31-N31)/3.14)*2,1)</f>
-        <v>259.8</v>
+        <f t="shared" ref="O31:O33" si="45">ROUND(SQRT((M31-N31)/3.14)*2,1)</f>
+        <v>649.5</v>
       </c>
       <c r="P31">
         <f>ROUND(C31/B31,2)</f>
-        <v>5.36</v>
-      </c>
-      <c r="Q31" s="6">
-        <f t="shared" ref="Q31" si="46">ROUND(K31/(C31/206),2)</f>
-        <v>0.48</v>
+        <v>5</v>
+      </c>
+      <c r="Q31" s="4">
+        <f t="shared" ref="Q31:Q33" si="46">ROUND(K31/(C31/206),2)</f>
+        <v>0.82</v>
       </c>
       <c r="R31" s="4">
-        <f t="shared" ref="R31" si="47">2*Q31</f>
-        <v>0.96</v>
+        <f t="shared" ref="R31:R33" si="47">2*Q31</f>
+        <v>1.64</v>
       </c>
       <c r="S31" s="5">
-        <f t="shared" ref="S31" si="48">3*Q31</f>
-        <v>1.44</v>
+        <f t="shared" ref="S31:S33" si="48">3*Q31</f>
+        <v>2.46</v>
       </c>
       <c r="T31" s="3">
-        <f t="shared" ref="T31" si="49">4*Q31</f>
-        <v>1.92</v>
-      </c>
-      <c r="U31" s="7">
-        <f t="shared" ref="U31" si="50">ROUND(O31^2*Q31^2*L31,1)</f>
-        <v>12440.9</v>
+        <f t="shared" ref="T31:T33" si="49">4*Q31</f>
+        <v>3.28</v>
+      </c>
+      <c r="U31" s="8">
+        <f t="shared" ref="U31:U33" si="50">ROUND(O31^2*Q31^2*L31,1)</f>
+        <v>269469.5</v>
       </c>
       <c r="V31" s="8">
-        <f t="shared" ref="V31" si="51">ROUND(O31^2*R31^2*L31,1)</f>
-        <v>49763.5</v>
+        <f t="shared" ref="V31:V33" si="51">ROUND(O31^2*R31^2*L31,1)</f>
+        <v>1077878</v>
       </c>
       <c r="W31" s="8">
-        <f t="shared" ref="W31" si="52">ROUND(O31^2*S31^2*L31,1)</f>
-        <v>111967.8</v>
+        <f t="shared" ref="W31:W33" si="52">ROUND(O31^2*S31^2*L31,1)</f>
+        <v>2425225.5</v>
       </c>
       <c r="X31" s="7">
-        <f t="shared" ref="X31" si="53">ROUND(O31^2*T31^2*L31,1)</f>
-        <v>199053.9</v>
+        <f t="shared" ref="X31:X33" si="53">ROUND(O31^2*T31^2*L31,1)</f>
+        <v>4311512</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32">
+        <v>750</v>
+      </c>
+      <c r="C32">
+        <f>C30*D32</f>
+        <v>2800</v>
+      </c>
+      <c r="D32">
+        <v>0.5</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F32" t="s">
+        <v>37</v>
+      </c>
+      <c r="G32" t="s">
+        <v>28</v>
+      </c>
+      <c r="H32">
+        <v>16</v>
+      </c>
+      <c r="I32">
+        <v>2048</v>
+      </c>
+      <c r="J32">
+        <v>2048</v>
+      </c>
+      <c r="K32">
+        <v>15</v>
+      </c>
+      <c r="L32" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="M32">
+        <f>ROUND(3.14*(B32/2)^2,1)</f>
+        <v>441562.5</v>
+      </c>
+      <c r="N32">
+        <f>ROUND(3.14*(B32*E32/2)^2,1)</f>
+        <v>110390.6</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="45"/>
+        <v>649.5</v>
+      </c>
+      <c r="P32">
+        <f>ROUND(C32/B32,2)</f>
+        <v>3.73</v>
+      </c>
+      <c r="Q32" s="10">
+        <f t="shared" si="46"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="R32" s="4">
+        <f t="shared" si="47"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="S32" s="13">
+        <f t="shared" si="48"/>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="T32" s="3">
+        <f t="shared" si="49"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="U32" s="8">
+        <f t="shared" si="50"/>
+        <v>484916.9</v>
+      </c>
+      <c r="V32" s="8">
+        <f t="shared" si="51"/>
+        <v>1939667.4</v>
+      </c>
+      <c r="W32" s="7">
+        <f t="shared" si="52"/>
+        <v>4364251.8</v>
+      </c>
+      <c r="X32" s="7">
+        <f t="shared" si="53"/>
+        <v>7758669.7999999998</v>
       </c>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B33">
-        <v>300</v>
+        <v>750</v>
       </c>
       <c r="C33">
-        <v>2400</v>
+        <f>C30*D33</f>
+        <v>1848</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="E33" s="2">
         <v>0.5</v>
       </c>
       <c r="F33" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="G33" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H33">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I33">
-        <v>4122</v>
+        <v>2048</v>
       </c>
       <c r="J33">
-        <v>2822</v>
+        <v>2048</v>
       </c>
       <c r="K33">
-        <v>4.63</v>
+        <v>15</v>
       </c>
       <c r="L33" s="2">
-        <v>0.75</v>
+        <v>0.95</v>
       </c>
       <c r="M33">
         <f>ROUND(3.14*(B33/2)^2,1)</f>
-        <v>70650</v>
+        <v>441562.5</v>
       </c>
       <c r="N33">
         <f>ROUND(3.14*(B33*E33/2)^2,1)</f>
-        <v>17662.5</v>
+        <v>110390.6</v>
       </c>
       <c r="O33">
-        <f>ROUND(SQRT((M33-N33)/3.14)*2,1)</f>
-        <v>259.8</v>
+        <f t="shared" si="45"/>
+        <v>649.5</v>
       </c>
       <c r="P33">
         <f>ROUND(C33/B33,2)</f>
+        <v>2.46</v>
+      </c>
+      <c r="Q33" s="8">
+        <f t="shared" si="46"/>
+        <v>1.67</v>
+      </c>
+      <c r="R33" s="12">
+        <f t="shared" si="47"/>
+        <v>3.34</v>
+      </c>
+      <c r="S33" s="11">
+        <f t="shared" si="48"/>
+        <v>5.01</v>
+      </c>
+      <c r="T33" s="12">
+        <f t="shared" si="49"/>
+        <v>6.68</v>
+      </c>
+      <c r="U33" s="8">
+        <f t="shared" si="50"/>
+        <v>1117673.3</v>
+      </c>
+      <c r="V33" s="7">
+        <f t="shared" si="51"/>
+        <v>4470693</v>
+      </c>
+      <c r="W33" s="7">
+        <f t="shared" si="52"/>
+        <v>10059059.300000001</v>
+      </c>
+      <c r="X33" s="7">
+        <f t="shared" si="53"/>
+        <v>17882772.100000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35">
+        <v>300</v>
+      </c>
+      <c r="C35">
+        <v>2400</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F35" t="s">
+        <v>23</v>
+      </c>
+      <c r="G35" t="s">
+        <v>24</v>
+      </c>
+      <c r="H35">
+        <v>16</v>
+      </c>
+      <c r="I35">
+        <v>6248</v>
+      </c>
+      <c r="J35">
+        <v>4176</v>
+      </c>
+      <c r="K35">
+        <v>3.75</v>
+      </c>
+      <c r="L35" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="M35">
+        <f>ROUND(3.14*(B35/2)^2,1)</f>
+        <v>70650</v>
+      </c>
+      <c r="N35">
+        <f>ROUND(3.14*(B35*E35/2)^2,1)</f>
+        <v>17662.5</v>
+      </c>
+      <c r="O35">
+        <f>ROUND(SQRT((M35-N35)/3.14)*2,1)</f>
+        <v>259.8</v>
+      </c>
+      <c r="P35">
+        <f>ROUND(C35/B35,2)</f>
         <v>8</v>
       </c>
-      <c r="Q33" s="3">
-        <f>ROUND(K33/(C33/206),2)</f>
-        <v>0.4</v>
-      </c>
-      <c r="R33" s="4">
-        <f>2*Q33</f>
-        <v>0.8</v>
-      </c>
-      <c r="S33" s="4">
-        <f>3*Q33</f>
-        <v>1.2000000000000002</v>
-      </c>
-      <c r="T33" s="4">
-        <f>4*Q33</f>
-        <v>1.6</v>
-      </c>
-      <c r="U33" s="7">
-        <f>ROUND(O33^2*Q33^2*L33,1)</f>
-        <v>8099.5</v>
-      </c>
-      <c r="V33" s="8">
-        <f>ROUND(O33^2*R33^2*L33,1)</f>
-        <v>32398.1</v>
-      </c>
-      <c r="W33" s="8">
-        <f>ROUND(O33^2*S33^2*L33,1)</f>
-        <v>72895.7</v>
-      </c>
-      <c r="X33" s="8">
-        <f>ROUND(O33^2*T33^2*L33,1)</f>
-        <v>129592.4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>31</v>
-      </c>
-      <c r="B34">
-        <v>300</v>
-      </c>
-      <c r="C34">
-        <f>C33*D34</f>
-        <v>1608</v>
-      </c>
-      <c r="D34">
-        <v>0.67</v>
-      </c>
-      <c r="E34" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="F34" t="s">
-        <v>26</v>
-      </c>
-      <c r="G34" t="s">
-        <v>24</v>
-      </c>
-      <c r="H34">
-        <v>14</v>
-      </c>
-      <c r="I34">
-        <v>4122</v>
-      </c>
-      <c r="J34">
-        <v>2822</v>
-      </c>
-      <c r="K34">
-        <v>4.63</v>
-      </c>
-      <c r="L34" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="M34">
-        <f>ROUND(3.14*(B34/2)^2,1)</f>
-        <v>70650</v>
-      </c>
-      <c r="N34">
-        <f>ROUND(3.14*(B34*E34/2)^2,1)</f>
-        <v>17662.5</v>
-      </c>
-      <c r="O34">
-        <f t="shared" ref="O34" si="54">ROUND(SQRT((M34-N34)/3.14)*2,1)</f>
-        <v>259.8</v>
-      </c>
-      <c r="P34">
-        <f>ROUND(C34/B34,2)</f>
-        <v>5.36</v>
-      </c>
-      <c r="Q34" s="6">
-        <f t="shared" ref="Q34" si="55">ROUND(K34/(C34/206),2)</f>
-        <v>0.59</v>
-      </c>
-      <c r="R34" s="4">
-        <f t="shared" ref="R34" si="56">2*Q34</f>
-        <v>1.18</v>
-      </c>
-      <c r="S34" s="5">
-        <f t="shared" ref="S34" si="57">3*Q34</f>
-        <v>1.77</v>
-      </c>
-      <c r="T34" s="3">
-        <f t="shared" ref="T34" si="58">4*Q34</f>
-        <v>2.36</v>
-      </c>
-      <c r="U34" s="7">
-        <f t="shared" ref="U34" si="59">ROUND(O34^2*Q34^2*L34,1)</f>
-        <v>17621.5</v>
-      </c>
-      <c r="V34" s="8">
-        <f t="shared" ref="V34" si="60">ROUND(O34^2*R34^2*L34,1)</f>
-        <v>70486.100000000006</v>
-      </c>
-      <c r="W34" s="8">
-        <f t="shared" ref="W34" si="61">ROUND(O34^2*S34^2*L34,1)</f>
-        <v>158593.79999999999</v>
-      </c>
-      <c r="X34" s="7">
-        <f t="shared" ref="X34" si="62">ROUND(O34^2*T34^2*L34,1)</f>
-        <v>281944.5</v>
+      <c r="Q35" s="3">
+        <f>ROUND(K35/(C35/206),2)</f>
+        <v>0.32</v>
+      </c>
+      <c r="R35" s="4">
+        <f>2*Q35</f>
+        <v>0.64</v>
+      </c>
+      <c r="S35" s="4">
+        <f>3*Q35</f>
+        <v>0.96</v>
+      </c>
+      <c r="T35" s="4">
+        <f>4*Q35</f>
+        <v>1.28</v>
+      </c>
+      <c r="U35" s="15">
+        <f>ROUND(O35^2*Q35^2*L35,1)</f>
+        <v>5529.3</v>
+      </c>
+      <c r="V35" s="8">
+        <f>ROUND(O35^2*R35^2*L35,1)</f>
+        <v>22117.1</v>
+      </c>
+      <c r="W35" s="8">
+        <f>ROUND(O35^2*S35^2*L35,1)</f>
+        <v>49763.5</v>
+      </c>
+      <c r="X35" s="8">
+        <f>ROUND(O35^2*T35^2*L35,1)</f>
+        <v>88468.4</v>
       </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B36">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="C36">
-        <v>1250</v>
+        <f>C35*D36</f>
+        <v>1608</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>0.67</v>
       </c>
       <c r="E36" s="2">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="F36" t="s">
         <v>23</v>
@@ -2992,308 +3095,567 @@
       </c>
       <c r="M36">
         <f>ROUND(3.14*(B36/2)^2,1)</f>
-        <v>49062.5</v>
+        <v>70650</v>
       </c>
       <c r="N36">
         <f>ROUND(3.14*(B36*E36/2)^2,1)</f>
-        <v>4415.6000000000004</v>
+        <v>17662.5</v>
       </c>
       <c r="O36">
-        <f>ROUND(SQRT((M36-N36)/3.14)*2,1)</f>
-        <v>238.5</v>
+        <f t="shared" ref="O36" si="54">ROUND(SQRT((M36-N36)/3.14)*2,1)</f>
+        <v>259.8</v>
       </c>
       <c r="P36">
         <f>ROUND(C36/B36,2)</f>
-        <v>5</v>
+        <v>5.36</v>
       </c>
       <c r="Q36" s="6">
-        <f>ROUND(K36/(C36/206),2)</f>
-        <v>0.62</v>
+        <f t="shared" ref="Q36" si="55">ROUND(K36/(C36/206),2)</f>
+        <v>0.48</v>
       </c>
       <c r="R36" s="4">
-        <f>2*Q36</f>
-        <v>1.24</v>
-      </c>
-      <c r="S36" s="4">
-        <f>3*Q36</f>
-        <v>1.8599999999999999</v>
-      </c>
-      <c r="T36" s="6">
-        <f>4*Q36</f>
-        <v>2.48</v>
+        <f t="shared" ref="R36" si="56">2*Q36</f>
+        <v>0.96</v>
+      </c>
+      <c r="S36" s="5">
+        <f t="shared" ref="S36" si="57">3*Q36</f>
+        <v>1.44</v>
+      </c>
+      <c r="T36" s="3">
+        <f t="shared" ref="T36" si="58">4*Q36</f>
+        <v>1.92</v>
       </c>
       <c r="U36" s="7">
-        <f>ROUND(O36^2*Q36^2*L36,1)</f>
-        <v>17492.400000000001</v>
+        <f t="shared" ref="U36" si="59">ROUND(O36^2*Q36^2*L36,1)</f>
+        <v>12440.9</v>
       </c>
       <c r="V36" s="8">
-        <f>ROUND(O36^2*R36^2*L36,1)</f>
-        <v>69969.7</v>
+        <f t="shared" ref="V36" si="60">ROUND(O36^2*R36^2*L36,1)</f>
+        <v>49763.5</v>
       </c>
       <c r="W36" s="8">
-        <f>ROUND(O36^2*S36^2*L36,1)</f>
-        <v>157431.9</v>
-      </c>
-      <c r="X36" s="8">
-        <f>ROUND(O36^2*T36^2*L36,1)</f>
-        <v>279878.90000000002</v>
+        <f t="shared" ref="W36" si="61">ROUND(O36^2*S36^2*L36,1)</f>
+        <v>111967.8</v>
+      </c>
+      <c r="X36" s="7">
+        <f t="shared" ref="X36" si="62">ROUND(O36^2*T36^2*L36,1)</f>
+        <v>199053.9</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>32</v>
-      </c>
-      <c r="B37">
-        <v>250</v>
-      </c>
-      <c r="C37">
-        <v>1000</v>
-      </c>
-      <c r="D37">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38">
+        <v>300</v>
+      </c>
+      <c r="C38">
+        <v>2400</v>
+      </c>
+      <c r="D38">
         <v>1</v>
       </c>
-      <c r="E37" s="2">
-        <v>0.35</v>
-      </c>
-      <c r="F37" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="G37" t="s">
+      <c r="E38" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F38" t="s">
+        <v>26</v>
+      </c>
+      <c r="G38" t="s">
         <v>24</v>
       </c>
-      <c r="H37">
-        <v>16</v>
-      </c>
-      <c r="I37">
-        <v>6248</v>
-      </c>
-      <c r="J37">
-        <v>4176</v>
-      </c>
-      <c r="K37">
-        <v>3.75</v>
-      </c>
-      <c r="L37" s="2">
+      <c r="H38">
+        <v>14</v>
+      </c>
+      <c r="I38">
+        <v>4122</v>
+      </c>
+      <c r="J38">
+        <v>2822</v>
+      </c>
+      <c r="K38">
+        <v>4.63</v>
+      </c>
+      <c r="L38" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="M38">
+        <f>ROUND(3.14*(B38/2)^2,1)</f>
+        <v>70650</v>
+      </c>
+      <c r="N38">
+        <f>ROUND(3.14*(B38*E38/2)^2,1)</f>
+        <v>17662.5</v>
+      </c>
+      <c r="O38">
+        <f>ROUND(SQRT((M38-N38)/3.14)*2,1)</f>
+        <v>259.8</v>
+      </c>
+      <c r="P38">
+        <f>ROUND(C38/B38,2)</f>
+        <v>8</v>
+      </c>
+      <c r="Q38" s="3">
+        <f>ROUND(K38/(C38/206),2)</f>
+        <v>0.4</v>
+      </c>
+      <c r="R38" s="4">
+        <f>2*Q38</f>
         <v>0.8</v>
       </c>
-      <c r="M37">
-        <f>ROUND(3.14*(B37/2)^2,1)</f>
-        <v>49062.5</v>
-      </c>
-      <c r="N37">
-        <f>ROUND(3.14*(B37*E37/2)^2,1)</f>
-        <v>6010.2</v>
-      </c>
-      <c r="O37">
-        <f t="shared" ref="O37" si="63">ROUND(SQRT((M37-N37)/3.14)*2,1)</f>
-        <v>234.2</v>
-      </c>
-      <c r="P37">
-        <f>ROUND(C37/B37,2)</f>
-        <v>4</v>
-      </c>
-      <c r="Q37" s="4">
-        <f t="shared" ref="Q37" si="64">ROUND(K37/(C37/206),2)</f>
-        <v>0.77</v>
-      </c>
-      <c r="R37" s="4">
-        <f t="shared" ref="R37" si="65">2*Q37</f>
-        <v>1.54</v>
-      </c>
-      <c r="S37" s="14">
-        <f t="shared" ref="S37" si="66">3*Q37</f>
-        <v>2.31</v>
-      </c>
-      <c r="T37" s="3">
-        <f t="shared" ref="T37" si="67">4*Q37</f>
-        <v>3.08</v>
-      </c>
-      <c r="U37" s="15">
-        <f t="shared" ref="U37" si="68">ROUND(O37^2*Q37^2*L37,1)</f>
-        <v>26016.3</v>
-      </c>
-      <c r="V37" s="8">
-        <f t="shared" ref="V37" si="69">ROUND(O37^2*R37^2*L37,1)</f>
-        <v>104065.1</v>
-      </c>
-      <c r="W37" s="8">
-        <f t="shared" ref="W37" si="70">ROUND(O37^2*S37^2*L37,1)</f>
-        <v>234146.5</v>
-      </c>
-      <c r="X37" s="7">
-        <f t="shared" ref="X37" si="71">ROUND(O37^2*T37^2*L37,1)</f>
-        <v>416260.5</v>
+      <c r="S38" s="4">
+        <f>3*Q38</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="T38" s="4">
+        <f>4*Q38</f>
+        <v>1.6</v>
+      </c>
+      <c r="U38" s="7">
+        <f>ROUND(O38^2*Q38^2*L38,1)</f>
+        <v>8099.5</v>
+      </c>
+      <c r="V38" s="8">
+        <f>ROUND(O38^2*R38^2*L38,1)</f>
+        <v>32398.1</v>
+      </c>
+      <c r="W38" s="8">
+        <f>ROUND(O38^2*S38^2*L38,1)</f>
+        <v>72895.7</v>
+      </c>
+      <c r="X38" s="8">
+        <f>ROUND(O38^2*T38^2*L38,1)</f>
+        <v>129592.4</v>
       </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B39">
-        <v>125</v>
+        <v>300</v>
       </c>
       <c r="C39">
-        <v>1000</v>
+        <f>C38*D39</f>
+        <v>1608</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>0.67</v>
       </c>
       <c r="E39" s="2">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F39" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G39" t="s">
         <v>24</v>
       </c>
       <c r="H39">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I39">
-        <v>6248</v>
+        <v>4122</v>
       </c>
       <c r="J39">
-        <v>4176</v>
+        <v>2822</v>
       </c>
       <c r="K39">
-        <v>3.75</v>
+        <v>4.63</v>
       </c>
       <c r="L39" s="2">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="M39">
         <f>ROUND(3.14*(B39/2)^2,1)</f>
-        <v>12265.6</v>
+        <v>70650</v>
       </c>
       <c r="N39">
         <f>ROUND(3.14*(B39*E39/2)^2,1)</f>
-        <v>0</v>
+        <v>17662.5</v>
       </c>
       <c r="O39">
-        <f>ROUND(SQRT((M39-N39)/3.14)*2,1)</f>
-        <v>125</v>
+        <f t="shared" ref="O39" si="63">ROUND(SQRT((M39-N39)/3.14)*2,1)</f>
+        <v>259.8</v>
       </c>
       <c r="P39">
         <f>ROUND(C39/B39,2)</f>
+        <v>5.36</v>
+      </c>
+      <c r="Q39" s="6">
+        <f t="shared" ref="Q39" si="64">ROUND(K39/(C39/206),2)</f>
+        <v>0.59</v>
+      </c>
+      <c r="R39" s="4">
+        <f t="shared" ref="R39" si="65">2*Q39</f>
+        <v>1.18</v>
+      </c>
+      <c r="S39" s="5">
+        <f t="shared" ref="S39" si="66">3*Q39</f>
+        <v>1.77</v>
+      </c>
+      <c r="T39" s="3">
+        <f t="shared" ref="T39" si="67">4*Q39</f>
+        <v>2.36</v>
+      </c>
+      <c r="U39" s="7">
+        <f t="shared" ref="U39" si="68">ROUND(O39^2*Q39^2*L39,1)</f>
+        <v>17621.5</v>
+      </c>
+      <c r="V39" s="8">
+        <f t="shared" ref="V39" si="69">ROUND(O39^2*R39^2*L39,1)</f>
+        <v>70486.100000000006</v>
+      </c>
+      <c r="W39" s="8">
+        <f t="shared" ref="W39" si="70">ROUND(O39^2*S39^2*L39,1)</f>
+        <v>158593.79999999999</v>
+      </c>
+      <c r="X39" s="7">
+        <f t="shared" ref="X39" si="71">ROUND(O39^2*T39^2*L39,1)</f>
+        <v>281944.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41">
+        <v>250</v>
+      </c>
+      <c r="C41">
+        <v>1250</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="F41" t="s">
+        <v>23</v>
+      </c>
+      <c r="G41" t="s">
+        <v>24</v>
+      </c>
+      <c r="H41">
+        <v>16</v>
+      </c>
+      <c r="I41">
+        <v>6248</v>
+      </c>
+      <c r="J41">
+        <v>4176</v>
+      </c>
+      <c r="K41">
+        <v>3.75</v>
+      </c>
+      <c r="L41" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="M41">
+        <f>ROUND(3.14*(B41/2)^2,1)</f>
+        <v>49062.5</v>
+      </c>
+      <c r="N41">
+        <f>ROUND(3.14*(B41*E41/2)^2,1)</f>
+        <v>4415.6000000000004</v>
+      </c>
+      <c r="O41">
+        <f>ROUND(SQRT((M41-N41)/3.14)*2,1)</f>
+        <v>238.5</v>
+      </c>
+      <c r="P41">
+        <f>ROUND(C41/B41,2)</f>
+        <v>5</v>
+      </c>
+      <c r="Q41" s="6">
+        <f>ROUND(K41/(C41/206),2)</f>
+        <v>0.62</v>
+      </c>
+      <c r="R41" s="4">
+        <f>2*Q41</f>
+        <v>1.24</v>
+      </c>
+      <c r="S41" s="4">
+        <f>3*Q41</f>
+        <v>1.8599999999999999</v>
+      </c>
+      <c r="T41" s="6">
+        <f>4*Q41</f>
+        <v>2.48</v>
+      </c>
+      <c r="U41" s="7">
+        <f>ROUND(O41^2*Q41^2*L41,1)</f>
+        <v>17492.400000000001</v>
+      </c>
+      <c r="V41" s="8">
+        <f>ROUND(O41^2*R41^2*L41,1)</f>
+        <v>69969.7</v>
+      </c>
+      <c r="W41" s="8">
+        <f>ROUND(O41^2*S41^2*L41,1)</f>
+        <v>157431.9</v>
+      </c>
+      <c r="X41" s="8">
+        <f>ROUND(O41^2*T41^2*L41,1)</f>
+        <v>279878.90000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42">
+        <v>250</v>
+      </c>
+      <c r="C42">
+        <v>1000</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="F42" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G42" t="s">
+        <v>24</v>
+      </c>
+      <c r="H42">
+        <v>16</v>
+      </c>
+      <c r="I42">
+        <v>6248</v>
+      </c>
+      <c r="J42">
+        <v>4176</v>
+      </c>
+      <c r="K42">
+        <v>3.75</v>
+      </c>
+      <c r="L42" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="M42">
+        <f>ROUND(3.14*(B42/2)^2,1)</f>
+        <v>49062.5</v>
+      </c>
+      <c r="N42">
+        <f>ROUND(3.14*(B42*E42/2)^2,1)</f>
+        <v>6010.2</v>
+      </c>
+      <c r="O42">
+        <f t="shared" ref="O42" si="72">ROUND(SQRT((M42-N42)/3.14)*2,1)</f>
+        <v>234.2</v>
+      </c>
+      <c r="P42">
+        <f>ROUND(C42/B42,2)</f>
+        <v>4</v>
+      </c>
+      <c r="Q42" s="4">
+        <f t="shared" ref="Q42" si="73">ROUND(K42/(C42/206),2)</f>
+        <v>0.77</v>
+      </c>
+      <c r="R42" s="4">
+        <f t="shared" ref="R42" si="74">2*Q42</f>
+        <v>1.54</v>
+      </c>
+      <c r="S42" s="14">
+        <f t="shared" ref="S42" si="75">3*Q42</f>
+        <v>2.31</v>
+      </c>
+      <c r="T42" s="3">
+        <f t="shared" ref="T42" si="76">4*Q42</f>
+        <v>3.08</v>
+      </c>
+      <c r="U42" s="15">
+        <f t="shared" ref="U42" si="77">ROUND(O42^2*Q42^2*L42,1)</f>
+        <v>26016.3</v>
+      </c>
+      <c r="V42" s="8">
+        <f t="shared" ref="V42" si="78">ROUND(O42^2*R42^2*L42,1)</f>
+        <v>104065.1</v>
+      </c>
+      <c r="W42" s="8">
+        <f t="shared" ref="W42" si="79">ROUND(O42^2*S42^2*L42,1)</f>
+        <v>234146.5</v>
+      </c>
+      <c r="X42" s="7">
+        <f t="shared" ref="X42" si="80">ROUND(O42^2*T42^2*L42,1)</f>
+        <v>416260.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44">
+        <v>125</v>
+      </c>
+      <c r="C44">
+        <v>1000</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44" s="2">
+        <v>0</v>
+      </c>
+      <c r="F44" t="s">
+        <v>23</v>
+      </c>
+      <c r="G44" t="s">
+        <v>24</v>
+      </c>
+      <c r="H44">
+        <v>16</v>
+      </c>
+      <c r="I44">
+        <v>6248</v>
+      </c>
+      <c r="J44">
+        <v>4176</v>
+      </c>
+      <c r="K44">
+        <v>3.75</v>
+      </c>
+      <c r="L44" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="M44">
+        <f>ROUND(3.14*(B44/2)^2,1)</f>
+        <v>12265.6</v>
+      </c>
+      <c r="N44">
+        <f>ROUND(3.14*(B44*E44/2)^2,1)</f>
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <f>ROUND(SQRT((M44-N44)/3.14)*2,1)</f>
+        <v>125</v>
+      </c>
+      <c r="P44">
+        <f>ROUND(C44/B44,2)</f>
         <v>8</v>
       </c>
-      <c r="Q39" s="10">
-        <f>ROUND(K39/(C39/206),2)</f>
+      <c r="Q44" s="10">
+        <f>ROUND(K44/(C44/206),2)</f>
         <v>0.77</v>
       </c>
-      <c r="R39" s="4">
-        <f>2*Q39</f>
+      <c r="R44" s="4">
+        <f>2*Q44</f>
         <v>1.54</v>
       </c>
-      <c r="S39" s="6">
-        <f>3*Q39</f>
+      <c r="S44" s="6">
+        <f>3*Q44</f>
         <v>2.31</v>
       </c>
-      <c r="T39" s="3">
-        <f>4*Q39</f>
+      <c r="T44" s="3">
+        <f>4*Q44</f>
         <v>3.08</v>
       </c>
-      <c r="U39" s="7">
-        <f>ROUND(O39^2*Q39^2*L39,1)</f>
+      <c r="U44" s="7">
+        <f>ROUND(O44^2*Q44^2*L44,1)</f>
         <v>7411.3</v>
       </c>
-      <c r="V39" s="8">
-        <f>ROUND(O39^2*R39^2*L39,1)</f>
+      <c r="V44" s="8">
+        <f>ROUND(O44^2*R44^2*L44,1)</f>
         <v>29645</v>
       </c>
-      <c r="W39" s="7">
-        <f>ROUND(O39^2*S39^2*L39,1)</f>
+      <c r="W44" s="7">
+        <f>ROUND(O44^2*S44^2*L44,1)</f>
         <v>66701.3</v>
       </c>
-      <c r="X39" s="7">
-        <f>ROUND(O39^2*T39^2*L39,1)</f>
+      <c r="X44" s="7">
+        <f>ROUND(O44^2*T44^2*L44,1)</f>
         <v>118580</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>33</v>
       </c>
-      <c r="B40">
+      <c r="B45">
         <v>125</v>
       </c>
-      <c r="C40">
+      <c r="C45">
         <v>800</v>
       </c>
-      <c r="D40">
+      <c r="D45">
         <v>0.8</v>
       </c>
-      <c r="E40" s="2">
+      <c r="E45" s="2">
         <v>0</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F45" t="s">
         <v>23</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G45" t="s">
         <v>24</v>
       </c>
-      <c r="H40">
+      <c r="H45">
         <v>16</v>
       </c>
-      <c r="I40">
+      <c r="I45">
         <v>6248</v>
       </c>
-      <c r="J40">
+      <c r="J45">
         <v>4176</v>
       </c>
-      <c r="K40">
+      <c r="K45">
         <v>3.75</v>
       </c>
-      <c r="L40" s="2">
+      <c r="L45" s="2">
         <v>0.8</v>
       </c>
-      <c r="M40">
-        <f>ROUND(3.14*(B40/2)^2,1)</f>
+      <c r="M45">
+        <f>ROUND(3.14*(B45/2)^2,1)</f>
         <v>12265.6</v>
       </c>
-      <c r="N40">
-        <f>ROUND(3.14*(B40*E40/2)^2,1)</f>
+      <c r="N45">
+        <f>ROUND(3.14*(B45*E45/2)^2,1)</f>
         <v>0</v>
       </c>
-      <c r="O40">
-        <f t="shared" ref="O40" si="72">ROUND(SQRT((M40-N40)/3.14)*2,1)</f>
+      <c r="O45">
+        <f t="shared" ref="O45" si="81">ROUND(SQRT((M45-N45)/3.14)*2,1)</f>
         <v>125</v>
       </c>
-      <c r="P40">
-        <f>ROUND(C40/B40,2)</f>
+      <c r="P45">
+        <f>ROUND(C45/B45,2)</f>
         <v>6.4</v>
       </c>
-      <c r="Q40" s="4">
-        <f t="shared" ref="Q40" si="73">ROUND(K40/(C40/206),2)</f>
+      <c r="Q45" s="4">
+        <f t="shared" ref="Q45" si="82">ROUND(K45/(C45/206),2)</f>
         <v>0.97</v>
       </c>
-      <c r="R40" s="4">
-        <f t="shared" ref="R40" si="74">2*Q40</f>
+      <c r="R45" s="4">
+        <f t="shared" ref="R45" si="83">2*Q45</f>
         <v>1.94</v>
       </c>
-      <c r="S40" s="13">
-        <f t="shared" ref="S40" si="75">3*Q40</f>
+      <c r="S45" s="13">
+        <f t="shared" ref="S45" si="84">3*Q45</f>
         <v>2.91</v>
       </c>
-      <c r="T40" s="3">
-        <f t="shared" ref="T40" si="76">4*Q40</f>
+      <c r="T45" s="3">
+        <f t="shared" ref="T45" si="85">4*Q45</f>
         <v>3.88</v>
       </c>
-      <c r="U40" s="8">
-        <f t="shared" ref="U40" si="77">ROUND(O40^2*Q40^2*L40,1)</f>
+      <c r="U45" s="8">
+        <f t="shared" ref="U45" si="86">ROUND(O45^2*Q45^2*L45,1)</f>
         <v>11761.3</v>
       </c>
-      <c r="V40" s="8">
-        <f t="shared" ref="V40" si="78">ROUND(O40^2*R40^2*L40,1)</f>
+      <c r="V45" s="8">
+        <f t="shared" ref="V45" si="87">ROUND(O45^2*R45^2*L45,1)</f>
         <v>47045</v>
       </c>
-      <c r="W40" s="7">
-        <f t="shared" ref="W40" si="79">ROUND(O40^2*S40^2*L40,1)</f>
+      <c r="W45" s="7">
+        <f t="shared" ref="W45" si="88">ROUND(O45^2*S45^2*L45,1)</f>
         <v>105851.3</v>
       </c>
-      <c r="X40" s="7">
-        <f t="shared" ref="X40" si="80">ROUND(O40^2*T40^2*L40,1)</f>
+      <c r="X45" s="7">
+        <f t="shared" ref="X45" si="89">ROUND(O45^2*T45^2*L45,1)</f>
         <v>188180</v>
       </c>
     </row>

</xml_diff>